<commit_message>
Updated with M.2 Connector
</commit_message>
<xml_diff>
--- a/E17-02-DCU/BOM-E17-02-DCU.xlsx
+++ b/E17-02-DCU/BOM-E17-02-DCU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
   <si>
     <t>Quantity</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>1727-1733-1-ND</t>
+  </si>
+  <si>
+    <t>A115899CT-ND</t>
+  </si>
+  <si>
+    <t>J6</t>
   </si>
 </sst>
 </file>
@@ -1123,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1601,6 +1607,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>